<commit_message>
Ajout correction sprint 2
</commit_message>
<xml_diff>
--- a/Equipe202.xlsx
+++ b/Equipe202.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24715"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="8_{50A2320D-A701-4D43-9EC9-8C1EC60D081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52645488-43D7-408E-ABEE-1F56887B8BB1}"/>
+  <xr:revisionPtr revIDLastSave="348" documentId="8_{50A2320D-A701-4D43-9EC9-8C1EC60D081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A85FE5B-F193-4FD3-8524-7D0AC833DC21}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="187">
   <si>
     <t>Fonct.</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Correcteur</t>
+  </si>
+  <si>
+    <t>Augustin</t>
   </si>
   <si>
     <t>1.1 Responsabilité</t>
@@ -121,6 +124,9 @@
     <t>isDebugModeActivated de CommandExecuterService; desactivateLetterMultiplicator et desactivateWordMultiplicator de Board inutiles</t>
   </si>
   <si>
+    <t>pending-games.component.ts:25, waiting-for-player.component.ts:20</t>
+  </si>
+  <si>
     <t>1.4 Accessibilité</t>
   </si>
   <si>
@@ -130,6 +136,9 @@
     <t>sendActionArgsMessage, validateAction ActionValidatorService; revert(), lettersToRemoveInRack dans PlaceLetter; createCommand, sendCommand, placeLetterFormatter, placeLetterArgVerifier, colArgVerifier, exchangeLetterArgVerifier de CommandParserService</t>
   </si>
   <si>
+    <t>abandon-button.component.ts:11 -&gt; Utiliser de l'injection privée, join-online-game.component.ts:15,pending-games.component.ts:18</t>
+  </si>
+  <si>
     <t>1.5 Valeur par défaut</t>
   </si>
   <si>
@@ -137,6 +146,9 @@
   </si>
   <si>
     <t>Bot on initialise dans constructeur alors que le reste hors</t>
+  </si>
+  <si>
+    <t>server-game.ts:42, server-game.ts:43, online-game.ts:gameState$$, game.ts:timerControls$$ + erreurs dans les autres classe</t>
   </si>
   <si>
     <t>Sous-total</t>
@@ -155,6 +167,9 @@
     <t xml:space="preserve">placeLetterFormatter() de CommandParserService et elle retourne une valeur (get a la place de place maybe); idem pour drawEmptyRackLetters, drawGameLetters de LetterBag; bot-crawler.ts : idem lineSplitter de ;getLettersOnLine alors que la fonction est void; wordCheck et crossCheck ne sont pas des bons noms: on s'attend  un boolean a retourner. </t>
   </si>
   <si>
+    <t xml:space="preserve">Quand une fonction retourne un booléen, une bonne pratique est de commencer le nom de functions par is.. ou has..., ou can.... </t>
+  </si>
+  <si>
     <t>2.2 Utilité</t>
   </si>
   <si>
@@ -162,6 +177,9 @@
   </si>
   <si>
     <t>validatePlaceLetter de ActionValidatorService; boardCrawler, lineSplitter, getLettersOnLine dans bot-crawler; formatAlternativeWord dans BotMessagesService; randomWordPicker dans Easybot; les fonctions de DictionryService; HeaderBarComponent:ngOnInit()</t>
+  </si>
+  <si>
+    <t>hearder-bar-component n'a pas besoin d'implémenter OnInit; La fonction formatPlaceLetter dans command-parser.service.ts peut être fragmentiée en au moins deux fonctions : une qui s'assure que tout est bon et une autre qui fait le placement quand tout est bon</t>
   </si>
   <si>
     <t>2.3 Nombre de paramètres</t>
@@ -174,12 +192,18 @@
     <t>placeLetterArgVerifier() de CommandParserService; boardCrawler,getLettersOnLine dns bot-crawler; initialDictionarySearch, subDictionarySearch, wholePartWordDictionarySearch, checkRightOfPlacedWord, dans DictionnarySErvice (-0.7)</t>
   </si>
   <si>
+    <t>UIPlace, BotCrawler, ValidWord et PlaceLetter prennent trop d'arguments dans leur constructeurs; canvas-drawer.ts:163</t>
+  </si>
+  <si>
     <t>2.4 Fonction pure</t>
   </si>
   <si>
     <t>Les fonctions sont pures lorsque possible. Les effets secondaires sont minimisés</t>
   </si>
   <si>
+    <t>chat-box.component.ts:66 La fonction aurait pu être pure au même titre que les autres fonctions</t>
+  </si>
+  <si>
     <t>2.5 Utilisation des paramètres</t>
   </si>
   <si>
@@ -192,6 +216,9 @@
     <t>Correcteur: Augustin</t>
   </si>
   <si>
+    <t>Sami</t>
+  </si>
+  <si>
     <t>3.1 Messages d'erreurs</t>
   </si>
   <si>
@@ -213,6 +240,9 @@
     <t>Tout code asynchrone (Promise, Observable ou Event) doit être géré adéquatement.</t>
   </si>
   <si>
+    <t>l87 dans command-executer.service: qu'arrive-til si le GET lance une erreur?: mettez un catchError -0.1</t>
+  </si>
+  <si>
     <t>4. Variables</t>
   </si>
   <si>
@@ -252,6 +282,9 @@
     <t>Les expression booléennes ne sont pas comparées à true ou false</t>
   </si>
   <si>
+    <t>canvas-drawer.ts:54</t>
+  </si>
+  <si>
     <t>5.2 Logique booléenne négative</t>
   </si>
   <si>
@@ -265,6 +298,9 @@
   </si>
   <si>
     <t>executeDebug() de CommandExecuterService operateur ternaire aurait fait l'affaire. idem pour createBot() dans BotCreatorService; idem pour doAction de Game; playAction idem dans EasyBot</t>
+  </si>
+  <si>
+    <t>place-letter.ts:104, place-letter.ts:111,ui-input-controller.service.ts:26,game-info.service.ts:toute la fin de fichier</t>
   </si>
   <si>
     <t>5.4 Prédicats</t>
@@ -298,6 +334,9 @@
     <t>Il y a une séparation entre le code Typescript, HTML et CSS.</t>
   </si>
   <si>
+    <t>evitez de faire du css dans du html (utilisation de style): game-page.component.html, chat-box.component.html -0.2</t>
+  </si>
+  <si>
     <t>6.3 Indentation et organisation</t>
   </si>
   <si>
@@ -319,6 +358,9 @@
     <t>Enlever le code mort : Exemple material-page</t>
   </si>
   <si>
+    <t>l64 et l68 dans game-socket-handler.service; l52 chat-box.component.ts; l180 messages-socket-handler.service -0.25</t>
+  </si>
+  <si>
     <t>6.6 Enums</t>
   </si>
   <si>
@@ -334,6 +376,9 @@
     <t>Les objets anonymes Javascript ne sont pas utilisés, des classes ou des interfaces sont utilisés</t>
   </si>
   <si>
+    <t>receiveRoll(args: unknow) le unknow est non necessaire car la methode est implementer juste dans ui-move et pas dans les autres classes 'filles' de UIAction -0.1. idem pour receiveRightClick -0.1. vous aurez pu les mettre comme optional parameters</t>
+  </si>
+  <si>
     <t>6.8 Duplication</t>
   </si>
   <si>
@@ -341,6 +386,9 @@
   </si>
   <si>
     <t>word-searcher.service.ts Beaucoup de duplication de code</t>
+  </si>
+  <si>
+    <t>validateOtherPlaceLetter et validateFirstPlaceLetter sont presque les meme: avoir un parametre optional pour hasNeighbour peut regler la duplication. getVerticalWordFromBoard et getHorizontalWordFromBoard dans ui-place;  goToBeginningOfWord et goToEndOfWord dans word-searcher.service: un extract method peut regler le probleme. validateMiddleOfPlacedWord et validateRightOfPlacedWord dans dictionary.service -1</t>
   </si>
   <si>
     <t>6.9 ESLint</t>
@@ -353,6 +401,9 @@
     <t>command-executer.service.ts:50 Il faut gérer l'execption; letter-creator.ts:36 letter-creator.ts:38 Mettre le tableau en dehors de la classe au même titre que les autres; classic-game.component.ts:29 Gérer l'execption</t>
   </si>
   <si>
+    <t>GameSocketHandlerService, OnlineChatHandlerService, NewOnlineGameSocketHandler: je comprend que vous mettez any sur le socket pour les tests mais vous auriez pu cast le SocketMock en any dans les tests et mettre eslint-disable dans les fichiers tests vu qu'on accepte ce comportement -0.25. l62 dans command-executer.service: vous auriez pu mettre un return statement a la place de rien -0.25</t>
+  </si>
+  <si>
     <t xml:space="preserve">6.10 Imbrication </t>
   </si>
   <si>
@@ -360,6 +411,9 @@
   </si>
   <si>
     <t>action-validator.service.ts:35 ; action-validator.service.ts:104 ; action-validator.service.ts:109 ; place-letter.ts:93</t>
+  </si>
+  <si>
+    <t>subDictionarySearch dans dictionary.service: le niveau d'imbrication peut etre eviter par l'utilisation de continue; (-0.1) action-validator L227-234 -0.1;</t>
   </si>
   <si>
     <t>6.11 Performance</t>
@@ -431,18 +485,12 @@
     <t>1.1 Point d'entrée de l'application</t>
   </si>
   <si>
-    <t>Sami</t>
-  </si>
-  <si>
     <t>1.2 Initialisation d'une nouvelle partie (mode solo)</t>
   </si>
   <si>
     <t>1.3 Mode de jeu classique - Joueur Virtuel débutant</t>
   </si>
   <si>
-    <t>Augustin</t>
-  </si>
-  <si>
     <t>Un très bon agent pour un début. Félicitations</t>
   </si>
   <si>
@@ -485,12 +533,21 @@
     <t>2.1 Mode multijoueur</t>
   </si>
   <si>
+    <t>Augustin &amp; Sami</t>
+  </si>
+  <si>
+    <t>Bug : Pas de lettres (Voir la capture ci-contre)</t>
+  </si>
+  <si>
     <t>2.2 Clavarder</t>
   </si>
   <si>
     <t>2.3 Validation des mots sur le serveur</t>
   </si>
   <si>
+    <t>Très bel effort de votre part de déplacer la logique dans le serveur</t>
+  </si>
+  <si>
     <t>2.4 Paramètres de partie (minuterie et mode aléatoire)</t>
   </si>
   <si>
@@ -500,10 +557,16 @@
     <t>2.6 Placer des lettres</t>
   </si>
   <si>
+    <t>On ne devrait pas être sensible à la direction quand on place un seul caractère.</t>
+  </si>
+  <si>
     <t>2.7 Échanger des lettres</t>
   </si>
   <si>
     <t>2.8 Abandonner une partie</t>
+  </si>
+  <si>
+    <t>Après l'abandon d'une partie, le joueur gagnant peut toujours placer des lettres</t>
   </si>
   <si>
     <t>2.9 Manipuler les lettres du chevalet</t>
@@ -1370,7 +1433,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="286">
+  <cellXfs count="288">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2036,6 +2099,12 @@
     <xf numFmtId="9" fontId="0" fillId="19" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2221,13 +2290,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="40 % - Accent1" xfId="4" builtinId="31"/>
-    <cellStyle name="40 % - Accent2" xfId="5" builtinId="35"/>
-    <cellStyle name="40 % - Accent3" xfId="6" builtinId="39"/>
+    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
-    <cellStyle name="Sortie" xfId="3" builtinId="21"/>
-    <cellStyle name="Texte explicatif" xfId="2" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2308,6 +2377,102 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F799770A-C6D8-471C-B132-F0EBE4064F29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10325100" y="7781925"/>
+          <a:ext cx="4572000" cy="3190875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14C3CCCB-0B92-4874-A886-B4B404D40203}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F799770A-C6D8-471C-B132-F0EBE4064F29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10325100" y="6067425"/>
+          <a:ext cx="4572000" cy="2343150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2610,7 +2775,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A3:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2674,22 +2839,22 @@
       </c>
       <c r="B5" s="214">
         <f>(Fonctionnalités!E36)</f>
-        <v>0</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="C5" s="215">
         <f>'Assurance Qualité'!F61</f>
-        <v>0</v>
+        <v>0.70650000000000002</v>
       </c>
       <c r="D5" s="215">
         <f t="shared" ref="D5:D6" si="0">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0</v>
+        <v>0.86339999999999995</v>
       </c>
       <c r="F5" s="13">
         <v>25</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" ref="G5:G7" si="1">D5*F5</f>
-        <v>0</v>
+        <v>21.584999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2741,8 +2906,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q61"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2761,36 +2926,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A2" s="246" t="s">
+      <c r="A2" s="248" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="246"/>
-      <c r="C2" s="246"/>
-      <c r="D2" s="246"/>
-      <c r="E2" s="246"/>
-      <c r="F2" s="246"/>
-      <c r="G2" s="246"/>
-      <c r="H2" s="246"/>
-      <c r="I2" s="246"/>
-      <c r="J2" s="246"/>
-      <c r="K2" s="246"/>
+      <c r="B2" s="248"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
+      <c r="G2" s="248"/>
+      <c r="H2" s="248"/>
+      <c r="I2" s="248"/>
+      <c r="J2" s="248"/>
+      <c r="K2" s="248"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
     </row>
     <row r="4" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A4" s="247" t="s">
+      <c r="A4" s="249" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="247"/>
-      <c r="C4" s="247"/>
-      <c r="D4" s="247"/>
-      <c r="E4" s="247"/>
-      <c r="F4" s="247"/>
-      <c r="G4" s="247"/>
-      <c r="H4" s="247"/>
-      <c r="I4" s="247"/>
-      <c r="J4" s="247"/>
-      <c r="K4" s="247"/>
+      <c r="B4" s="249"/>
+      <c r="C4" s="249"/>
+      <c r="D4" s="249"/>
+      <c r="E4" s="249"/>
+      <c r="F4" s="249"/>
+      <c r="G4" s="249"/>
+      <c r="H4" s="249"/>
+      <c r="I4" s="249"/>
+      <c r="J4" s="249"/>
+      <c r="K4" s="249"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
@@ -2810,36 +2975,36 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A6" s="239" t="s">
+      <c r="A6" s="241" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="251" t="s">
+      <c r="B6" s="253" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="241" t="s">
+      <c r="C6" s="243" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="242"/>
-      <c r="E6" s="242"/>
-      <c r="F6" s="243" t="s">
+      <c r="D6" s="244"/>
+      <c r="E6" s="244"/>
+      <c r="F6" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="244"/>
-      <c r="H6" s="245"/>
-      <c r="I6" s="248" t="s">
+      <c r="G6" s="246"/>
+      <c r="H6" s="247"/>
+      <c r="I6" s="250" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="249"/>
-      <c r="K6" s="250"/>
+      <c r="J6" s="251"/>
+      <c r="K6" s="252"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="237"/>
-      <c r="O6" s="238"/>
-      <c r="P6" s="238"/>
+      <c r="N6" s="239"/>
+      <c r="O6" s="240"/>
+      <c r="P6" s="240"/>
     </row>
     <row r="7" spans="1:17" ht="19.5" thickBot="1">
-      <c r="A7" s="240"/>
-      <c r="B7" s="252"/>
+      <c r="A7" s="242"/>
+      <c r="B7" s="254"/>
       <c r="C7" s="22" t="s">
         <v>14</v>
       </c>
@@ -2874,35 +3039,37 @@
       <c r="P7" s="219"/>
       <c r="Q7" s="219"/>
     </row>
-    <row r="8" spans="1:17" s="20" customFormat="1" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A8" s="229" t="s">
+    <row r="8" spans="1:17" s="20" customFormat="1" ht="18.399999999999999" customHeight="1">
+      <c r="A8" s="231" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="230"/>
-      <c r="C8" s="225" t="s">
+      <c r="B8" s="232"/>
+      <c r="C8" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="226"/>
+      <c r="D8" s="228"/>
       <c r="E8" s="60"/>
-      <c r="F8" s="225" t="s">
+      <c r="F8" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="226"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="225" t="s">
+      <c r="G8" s="228"/>
+      <c r="H8" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="226"/>
+      <c r="J8" s="228"/>
       <c r="K8" s="60"/>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
     </row>
-    <row r="9" spans="1:17" ht="60">
+    <row r="9" spans="1:17" ht="45">
       <c r="A9" s="78" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="51">
         <v>0.6</v>
@@ -2911,9 +3078,11 @@
         <v>3</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="53"/>
+        <v>21</v>
+      </c>
+      <c r="F9" s="53">
+        <v>1</v>
+      </c>
       <c r="G9" s="48">
         <v>3</v>
       </c>
@@ -2928,10 +3097,10 @@
     </row>
     <row r="10" spans="1:17" ht="45">
       <c r="A10" s="21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="35">
         <v>1</v>
@@ -2940,7 +3109,9 @@
         <v>2</v>
       </c>
       <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
+      <c r="F10" s="37">
+        <v>1</v>
+      </c>
       <c r="G10" s="33">
         <v>2</v>
       </c>
@@ -2953,12 +3124,12 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:17" ht="135">
+    <row r="11" spans="1:17" ht="105">
       <c r="A11" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="35">
         <v>0.7</v>
@@ -2967,13 +3138,17 @@
         <v>3</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="37"/>
+        <v>26</v>
+      </c>
+      <c r="F11" s="37">
+        <v>0.75</v>
+      </c>
       <c r="G11" s="33">
         <v>3</v>
       </c>
-      <c r="H11" s="38"/>
+      <c r="H11" s="38" t="s">
+        <v>27</v>
+      </c>
       <c r="I11" s="39"/>
       <c r="J11" s="34">
         <v>3</v>
@@ -2982,12 +3157,12 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="255">
+    <row r="12" spans="1:17" ht="195">
       <c r="A12" s="21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="35">
         <v>0</v>
@@ -2996,13 +3171,17 @@
         <v>2</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="37"/>
+        <v>30</v>
+      </c>
+      <c r="F12" s="37">
+        <v>0</v>
+      </c>
       <c r="G12" s="33">
         <v>2</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="38" t="s">
+        <v>31</v>
+      </c>
       <c r="I12" s="39"/>
       <c r="J12" s="34">
         <v>2</v>
@@ -3011,12 +3190,12 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:17" ht="45">
+    <row r="13" spans="1:17" ht="90">
       <c r="A13" s="21" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C13" s="35">
         <v>0.9</v>
@@ -3025,13 +3204,17 @@
         <v>4</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="37"/>
+        <v>34</v>
+      </c>
+      <c r="F13" s="37">
+        <v>0</v>
+      </c>
       <c r="G13" s="33">
         <v>4</v>
       </c>
-      <c r="H13" s="38"/>
+      <c r="H13" s="38" t="s">
+        <v>35</v>
+      </c>
       <c r="I13" s="39"/>
       <c r="J13" s="34">
         <v>4</v>
@@ -3041,10 +3224,10 @@
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:17" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A14" s="227" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="228"/>
+      <c r="A14" s="229" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="230"/>
       <c r="C14" s="87">
         <f>SUMPRODUCT(C9:C13,D9:D13)</f>
         <v>9.5</v>
@@ -3056,7 +3239,7 @@
       <c r="E14" s="89"/>
       <c r="F14" s="90">
         <f>SUMPRODUCT(F9:F13,G9:G13)</f>
-        <v>0</v>
+        <v>7.25</v>
       </c>
       <c r="G14" s="91">
         <f>SUM(G9:G13)</f>
@@ -3075,35 +3258,37 @@
       <c r="L14" s="96"/>
       <c r="M14" s="96"/>
     </row>
-    <row r="15" spans="1:17" s="20" customFormat="1" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A15" s="234" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="235"/>
-      <c r="C15" s="225" t="s">
+    <row r="15" spans="1:17" s="20" customFormat="1" ht="18.399999999999999" customHeight="1">
+      <c r="A15" s="236" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="237"/>
+      <c r="C15" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="226"/>
+      <c r="D15" s="228"/>
       <c r="E15" s="60"/>
-      <c r="F15" s="225" t="s">
+      <c r="F15" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="226"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="225" t="s">
+      <c r="G15" s="228"/>
+      <c r="H15" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="226"/>
+      <c r="J15" s="228"/>
       <c r="K15" s="60"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:17" ht="315">
+    <row r="16" spans="1:17" ht="255">
       <c r="A16" s="78" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B16" s="79" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C16" s="62">
         <v>0</v>
@@ -3112,13 +3297,17 @@
         <v>2</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="68"/>
+        <v>40</v>
+      </c>
+      <c r="F16" s="68">
+        <v>0.75</v>
+      </c>
       <c r="G16" s="69">
         <v>2</v>
       </c>
-      <c r="H16" s="70"/>
+      <c r="H16" s="70" t="s">
+        <v>41</v>
+      </c>
       <c r="I16" s="74"/>
       <c r="J16" s="75">
         <v>2</v>
@@ -3127,12 +3316,12 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" ht="180">
+    <row r="17" spans="1:13" ht="195">
       <c r="A17" s="21" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C17" s="45">
         <v>0</v>
@@ -3141,13 +3330,17 @@
         <v>3</v>
       </c>
       <c r="E17" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="71"/>
+        <v>44</v>
+      </c>
+      <c r="F17" s="71">
+        <v>0.25</v>
+      </c>
       <c r="G17" s="42">
         <v>3</v>
       </c>
-      <c r="H17" s="72"/>
+      <c r="H17" s="72" t="s">
+        <v>45</v>
+      </c>
       <c r="I17" s="77"/>
       <c r="J17" s="44">
         <v>3</v>
@@ -3156,12 +3349,12 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" ht="210">
+    <row r="18" spans="1:13" ht="165">
       <c r="A18" s="21" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C18" s="45">
         <v>0.3</v>
@@ -3170,13 +3363,17 @@
         <v>3</v>
       </c>
       <c r="E18" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="71"/>
+        <v>48</v>
+      </c>
+      <c r="F18" s="71">
+        <v>0</v>
+      </c>
       <c r="G18" s="42">
         <v>3</v>
       </c>
-      <c r="H18" s="72"/>
+      <c r="H18" s="72" t="s">
+        <v>49</v>
+      </c>
       <c r="I18" s="77"/>
       <c r="J18" s="44">
         <v>3</v>
@@ -3185,12 +3382,12 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" ht="75">
       <c r="A19" s="21" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C19" s="45">
         <v>1</v>
@@ -3199,11 +3396,15 @@
         <v>3</v>
       </c>
       <c r="E19" s="65"/>
-      <c r="F19" s="71"/>
+      <c r="F19" s="71">
+        <v>0.75</v>
+      </c>
       <c r="G19" s="42">
         <v>3</v>
       </c>
-      <c r="H19" s="72"/>
+      <c r="H19" s="72" t="s">
+        <v>52</v>
+      </c>
       <c r="I19" s="77"/>
       <c r="J19" s="44">
         <v>3</v>
@@ -3214,10 +3415,10 @@
     </row>
     <row r="20" spans="1:13" ht="30">
       <c r="A20" s="21" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C20" s="45">
         <v>1</v>
@@ -3226,7 +3427,9 @@
         <v>2</v>
       </c>
       <c r="E20" s="65"/>
-      <c r="F20" s="71"/>
+      <c r="F20" s="71">
+        <v>1</v>
+      </c>
       <c r="G20" s="42">
         <v>2</v>
       </c>
@@ -3240,10 +3443,10 @@
       <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A21" s="236" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="233"/>
+      <c r="A21" s="238" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="235"/>
       <c r="C21" s="98">
         <f>SUMPRODUCT(C16:C20,D16:D20)</f>
         <v>5.9</v>
@@ -3255,7 +3458,7 @@
       <c r="E21" s="100"/>
       <c r="F21" s="101">
         <f>SUMPRODUCT(F16:F20,G16:G20)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="G21" s="102">
         <f>SUM(G16:G20)</f>
@@ -3275,34 +3478,36 @@
       <c r="M21" s="96"/>
     </row>
     <row r="22" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A22" s="229" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="230"/>
-      <c r="C22" s="225" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="226"/>
+      <c r="A22" s="231" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="232"/>
+      <c r="C22" s="227" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="228"/>
       <c r="E22" s="60"/>
-      <c r="F22" s="225" t="s">
+      <c r="F22" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="226"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="225" t="s">
+      <c r="G22" s="228"/>
+      <c r="H22" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="226"/>
+      <c r="J22" s="228"/>
       <c r="K22" s="60"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" ht="60">
       <c r="A23" s="80" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B23" s="81" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C23" s="84">
         <v>1</v>
@@ -3311,7 +3516,9 @@
         <v>2</v>
       </c>
       <c r="E23" s="86"/>
-      <c r="F23" s="109"/>
+      <c r="F23" s="109">
+        <v>1</v>
+      </c>
       <c r="G23" s="110">
         <v>2</v>
       </c>
@@ -3326,10 +3533,10 @@
     </row>
     <row r="24" spans="1:13" ht="120">
       <c r="A24" s="82" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B24" s="83" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C24" s="45">
         <v>0</v>
@@ -3338,9 +3545,11 @@
         <v>1</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="71"/>
+        <v>62</v>
+      </c>
+      <c r="F24" s="71">
+        <v>1</v>
+      </c>
       <c r="G24" s="42">
         <v>1</v>
       </c>
@@ -3355,10 +3564,10 @@
     </row>
     <row r="25" spans="1:13" ht="120">
       <c r="A25" s="82" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B25" s="83" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C25" s="45">
         <v>0</v>
@@ -3367,13 +3576,17 @@
         <v>1</v>
       </c>
       <c r="E25" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="71"/>
+        <v>62</v>
+      </c>
+      <c r="F25" s="71">
+        <v>0.9</v>
+      </c>
       <c r="G25" s="42">
         <v>1</v>
       </c>
-      <c r="H25" s="72"/>
+      <c r="H25" s="72" t="s">
+        <v>65</v>
+      </c>
       <c r="I25" s="77"/>
       <c r="J25" s="44">
         <v>1</v>
@@ -3383,10 +3596,10 @@
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A26" s="232" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="233"/>
+      <c r="A26" s="234" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="235"/>
       <c r="C26" s="87">
         <f>SUMPRODUCT(C23:C25,D23:D25)</f>
         <v>2</v>
@@ -3398,7 +3611,7 @@
       <c r="E26" s="89"/>
       <c r="F26" s="101">
         <f>SUMPRODUCT(F23:F25,G23:G25)</f>
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="G26" s="102">
         <f>SUM(G23:G25)</f>
@@ -3417,35 +3630,37 @@
       <c r="L26" s="96"/>
       <c r="M26" s="96"/>
     </row>
-    <row r="27" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A27" s="229" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="230"/>
-      <c r="C27" s="225" t="s">
+    <row r="27" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A27" s="231" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="232"/>
+      <c r="C27" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="226"/>
+      <c r="D27" s="228"/>
       <c r="E27" s="60"/>
-      <c r="F27" s="225" t="s">
+      <c r="F27" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="226"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="225" t="s">
+      <c r="G27" s="228"/>
+      <c r="H27" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="226"/>
+      <c r="J27" s="228"/>
       <c r="K27" s="60"/>
       <c r="L27" s="16"/>
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:13" ht="45">
       <c r="A28" s="120" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B28" s="121" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C28" s="112">
         <v>1</v>
@@ -3454,7 +3669,9 @@
         <v>2</v>
       </c>
       <c r="E28" s="113"/>
-      <c r="F28" s="107"/>
+      <c r="F28" s="107">
+        <v>1</v>
+      </c>
       <c r="G28" s="66">
         <v>2</v>
       </c>
@@ -3469,10 +3686,10 @@
     </row>
     <row r="29" spans="1:13" ht="30">
       <c r="A29" s="56" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B29" s="57" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C29" s="45">
         <v>1</v>
@@ -3481,7 +3698,9 @@
         <v>2</v>
       </c>
       <c r="E29" s="65"/>
-      <c r="F29" s="71"/>
+      <c r="F29" s="71">
+        <v>1</v>
+      </c>
       <c r="G29" s="42">
         <v>2</v>
       </c>
@@ -3496,10 +3715,10 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="21" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B30" s="57" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C30" s="45">
         <v>1</v>
@@ -3508,7 +3727,9 @@
         <v>2</v>
       </c>
       <c r="E30" s="65"/>
-      <c r="F30" s="71"/>
+      <c r="F30" s="71">
+        <v>1</v>
+      </c>
       <c r="G30" s="42">
         <v>2</v>
       </c>
@@ -3521,12 +3742,12 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" ht="225">
+    <row r="31" spans="1:13" ht="165">
       <c r="A31" s="21" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B31" s="57" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C31" s="45">
         <v>0</v>
@@ -3535,9 +3756,11 @@
         <v>3</v>
       </c>
       <c r="E31" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" s="71"/>
+        <v>75</v>
+      </c>
+      <c r="F31" s="71">
+        <v>1</v>
+      </c>
       <c r="G31" s="42">
         <v>3</v>
       </c>
@@ -3551,10 +3774,10 @@
       <c r="M31" s="6"/>
     </row>
     <row r="32" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A32" s="227" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="228"/>
+      <c r="A32" s="229" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="230"/>
       <c r="C32" s="87">
         <f>SUMPRODUCT(C28:C31,D28:D31)</f>
         <v>6</v>
@@ -3566,7 +3789,7 @@
       <c r="E32" s="89"/>
       <c r="F32" s="90">
         <f>SUMPRODUCT(F28:F31,G28:G31)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G32" s="91">
         <f>SUM(G28:G31)</f>
@@ -3585,21 +3808,23 @@
       <c r="L32" s="96"/>
       <c r="M32" s="96"/>
     </row>
-    <row r="33" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A33" s="229" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="231"/>
-      <c r="C33" s="225" t="s">
+    <row r="33" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A33" s="231" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="233"/>
+      <c r="C33" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="226"/>
+      <c r="D33" s="228"/>
       <c r="E33" s="60"/>
-      <c r="F33" s="225" t="s">
+      <c r="F33" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="226"/>
-      <c r="H33" s="60"/>
+      <c r="G33" s="228"/>
+      <c r="H33" s="60" t="s">
+        <v>18</v>
+      </c>
       <c r="I33" s="58" t="s">
         <v>17</v>
       </c>
@@ -3610,10 +3835,10 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="120" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B34" s="79" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C34" s="112">
         <v>1</v>
@@ -3622,11 +3847,15 @@
         <v>1</v>
       </c>
       <c r="E34" s="113"/>
-      <c r="F34" s="107"/>
+      <c r="F34" s="107">
+        <v>0.5</v>
+      </c>
       <c r="G34" s="66">
         <v>1</v>
       </c>
-      <c r="H34" s="108"/>
+      <c r="H34" s="108" t="s">
+        <v>79</v>
+      </c>
       <c r="I34" s="118"/>
       <c r="J34" s="73">
         <v>1</v>
@@ -3637,10 +3866,10 @@
     </row>
     <row r="35" spans="1:13" ht="30">
       <c r="A35" s="56" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C35" s="45">
         <v>1</v>
@@ -3649,7 +3878,9 @@
         <v>1</v>
       </c>
       <c r="E35" s="65"/>
-      <c r="F35" s="71"/>
+      <c r="F35" s="71">
+        <v>1</v>
+      </c>
       <c r="G35" s="42">
         <v>1</v>
       </c>
@@ -3662,12 +3893,12 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" ht="165">
+    <row r="36" spans="1:13" ht="135">
       <c r="A36" s="21" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C36" s="45">
         <v>0.6</v>
@@ -3676,13 +3907,17 @@
         <v>3</v>
       </c>
       <c r="E36" s="65" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="71"/>
+        <v>84</v>
+      </c>
+      <c r="F36" s="71">
+        <v>0</v>
+      </c>
       <c r="G36" s="42">
         <v>3</v>
       </c>
-      <c r="H36" s="72"/>
+      <c r="H36" s="72" t="s">
+        <v>85</v>
+      </c>
       <c r="I36" s="77"/>
       <c r="J36" s="44">
         <v>3</v>
@@ -3691,12 +3926,12 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="1:13" ht="45">
+    <row r="37" spans="1:13" ht="30">
       <c r="A37" s="21" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C37" s="45">
         <v>0.9</v>
@@ -3705,9 +3940,11 @@
         <v>3</v>
       </c>
       <c r="E37" s="65" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="71"/>
+        <v>88</v>
+      </c>
+      <c r="F37" s="71">
+        <v>1</v>
+      </c>
       <c r="G37" s="42">
         <v>3</v>
       </c>
@@ -3721,10 +3958,10 @@
       <c r="M37" s="6"/>
     </row>
     <row r="38" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A38" s="227" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="228"/>
+      <c r="A38" s="229" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="230"/>
       <c r="C38" s="122">
         <f>SUMPRODUCT(C34:C37,D34:D37)</f>
         <v>6.5</v>
@@ -3736,7 +3973,7 @@
       <c r="E38" s="89"/>
       <c r="F38" s="123">
         <f>SUMPRODUCT(F34:F37,G34:G37)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="G38" s="91">
         <f>SUM(G34:G37)</f>
@@ -3756,34 +3993,36 @@
       <c r="M38" s="96"/>
     </row>
     <row r="39" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A39" s="229" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" s="230"/>
-      <c r="C39" s="225" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="226"/>
+      <c r="A39" s="231" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="232"/>
+      <c r="C39" s="227" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="228"/>
       <c r="E39" s="59"/>
-      <c r="F39" s="225" t="s">
+      <c r="F39" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="226"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="225" t="s">
+      <c r="G39" s="228"/>
+      <c r="H39" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="J39" s="226"/>
+      <c r="J39" s="228"/>
       <c r="K39" s="60"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
     </row>
     <row r="40" spans="1:13" ht="60">
       <c r="A40" s="78" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B40" s="79" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C40" s="84">
         <v>0</v>
@@ -3792,9 +4031,11 @@
         <v>1</v>
       </c>
       <c r="E40" s="86" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" s="109"/>
+        <v>93</v>
+      </c>
+      <c r="F40" s="109">
+        <v>1</v>
+      </c>
       <c r="G40" s="110">
         <v>1</v>
       </c>
@@ -3807,12 +4048,12 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="1:13" ht="30">
+    <row r="41" spans="1:13" ht="90">
       <c r="A41" s="21" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C41" s="45">
         <v>1</v>
@@ -3821,11 +4062,15 @@
         <v>4</v>
       </c>
       <c r="E41" s="65"/>
-      <c r="F41" s="71"/>
+      <c r="F41" s="71">
+        <v>0.8</v>
+      </c>
       <c r="G41" s="42">
         <v>4</v>
       </c>
-      <c r="H41" s="72"/>
+      <c r="H41" s="72" t="s">
+        <v>96</v>
+      </c>
       <c r="I41" s="77"/>
       <c r="J41" s="44">
         <v>4</v>
@@ -3836,10 +4081,10 @@
     </row>
     <row r="42" spans="1:13" ht="30">
       <c r="A42" s="21" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C42" s="45">
         <v>1</v>
@@ -3848,7 +4093,9 @@
         <v>3</v>
       </c>
       <c r="E42" s="65"/>
-      <c r="F42" s="71"/>
+      <c r="F42" s="71">
+        <v>1</v>
+      </c>
       <c r="G42" s="42">
         <v>3</v>
       </c>
@@ -3863,10 +4110,10 @@
     </row>
     <row r="43" spans="1:13" ht="45">
       <c r="A43" s="21" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C43" s="45">
         <v>1</v>
@@ -3875,7 +4122,9 @@
         <v>2</v>
       </c>
       <c r="E43" s="65"/>
-      <c r="F43" s="71"/>
+      <c r="F43" s="71">
+        <v>1</v>
+      </c>
       <c r="G43" s="42">
         <v>2</v>
       </c>
@@ -3887,12 +4136,12 @@
       <c r="K43" s="46"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="1:13" ht="45">
+    <row r="44" spans="1:13" ht="90">
       <c r="A44" s="21" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C44" s="35">
         <v>1</v>
@@ -3901,13 +4150,17 @@
         <v>2</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" s="37"/>
+        <v>103</v>
+      </c>
+      <c r="F44" s="37">
+        <v>0.75</v>
+      </c>
       <c r="G44" s="33">
         <v>2</v>
       </c>
-      <c r="H44" s="38"/>
+      <c r="H44" s="38" t="s">
+        <v>104</v>
+      </c>
       <c r="I44" s="39"/>
       <c r="J44" s="34">
         <v>2</v>
@@ -3918,10 +4171,10 @@
     </row>
     <row r="45" spans="1:13" ht="45">
       <c r="A45" s="21" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C45" s="35">
         <v>0</v>
@@ -3930,9 +4183,11 @@
         <v>3</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" s="37"/>
+        <v>107</v>
+      </c>
+      <c r="F45" s="37">
+        <v>1</v>
+      </c>
       <c r="G45" s="33">
         <v>3</v>
       </c>
@@ -3945,12 +4200,12 @@
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="1:13" ht="30">
+    <row r="46" spans="1:13" ht="180">
       <c r="A46" s="21" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C46" s="45">
         <v>1</v>
@@ -3959,11 +4214,15 @@
         <v>3</v>
       </c>
       <c r="E46" s="65"/>
-      <c r="F46" s="71"/>
+      <c r="F46" s="71">
+        <v>0.8</v>
+      </c>
       <c r="G46" s="42">
         <v>3</v>
       </c>
-      <c r="H46" s="72"/>
+      <c r="H46" s="72" t="s">
+        <v>110</v>
+      </c>
       <c r="I46" s="77"/>
       <c r="J46" s="44">
         <v>3</v>
@@ -3972,12 +4231,12 @@
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="1:13" ht="45">
+    <row r="47" spans="1:13" ht="300">
       <c r="A47" s="21" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="C47" s="45">
         <v>0.5</v>
@@ -3986,13 +4245,17 @@
         <v>6</v>
       </c>
       <c r="E47" s="65" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="71"/>
+        <v>113</v>
+      </c>
+      <c r="F47" s="71">
+        <v>0</v>
+      </c>
       <c r="G47" s="42">
         <v>6</v>
       </c>
-      <c r="H47" s="72"/>
+      <c r="H47" s="72" t="s">
+        <v>114</v>
+      </c>
       <c r="I47" s="77"/>
       <c r="J47" s="44">
         <v>6</v>
@@ -4001,12 +4264,12 @@
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="1:13" ht="150">
+    <row r="48" spans="1:13" ht="285">
       <c r="A48" s="21" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="C48" s="45">
         <v>0.6</v>
@@ -4015,13 +4278,17 @@
         <v>8</v>
       </c>
       <c r="E48" s="65" t="s">
-        <v>101</v>
-      </c>
-      <c r="F48" s="71"/>
+        <v>117</v>
+      </c>
+      <c r="F48" s="71">
+        <v>0.5</v>
+      </c>
       <c r="G48" s="42">
         <v>8</v>
       </c>
-      <c r="H48" s="72"/>
+      <c r="H48" s="72" t="s">
+        <v>118</v>
+      </c>
       <c r="I48" s="77"/>
       <c r="J48" s="44">
         <v>8</v>
@@ -4030,12 +4297,12 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="1:13" ht="90">
+    <row r="49" spans="1:13" ht="105">
       <c r="A49" s="21" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C49" s="45">
         <v>0</v>
@@ -4044,13 +4311,17 @@
         <v>6</v>
       </c>
       <c r="E49" s="65" t="s">
-        <v>104</v>
-      </c>
-      <c r="F49" s="71"/>
+        <v>121</v>
+      </c>
+      <c r="F49" s="71">
+        <v>0.9</v>
+      </c>
       <c r="G49" s="42">
         <v>6</v>
       </c>
-      <c r="H49" s="72"/>
+      <c r="H49" s="72" t="s">
+        <v>122</v>
+      </c>
       <c r="I49" s="77"/>
       <c r="J49" s="44">
         <v>6</v>
@@ -4061,10 +4332,10 @@
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="21" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C50" s="45">
         <v>1</v>
@@ -4073,7 +4344,9 @@
         <v>3</v>
       </c>
       <c r="E50" s="65"/>
-      <c r="F50" s="71"/>
+      <c r="F50" s="71">
+        <v>1</v>
+      </c>
       <c r="G50" s="42">
         <v>3</v>
       </c>
@@ -4086,11 +4359,11 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
     </row>
-    <row r="51" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A51" s="227" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" s="228"/>
+    <row r="51" spans="1:13" s="97" customFormat="1" ht="15.75">
+      <c r="A51" s="229" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="230"/>
       <c r="C51" s="132">
         <f>SUMPRODUCT(C40:C50,D40:D50)</f>
         <v>24.8</v>
@@ -4102,7 +4375,7 @@
       <c r="E51" s="100"/>
       <c r="F51" s="123">
         <f>SUMPRODUCT(F40:F50,G40:G50)</f>
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="G51" s="91">
         <f>SUM(G40:G50)</f>
@@ -4121,35 +4394,37 @@
       <c r="L51" s="96"/>
       <c r="M51" s="96"/>
     </row>
-    <row r="52" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A52" s="229" t="s">
-        <v>107</v>
-      </c>
-      <c r="B52" s="231"/>
-      <c r="C52" s="225" t="s">
-        <v>78</v>
-      </c>
-      <c r="D52" s="226"/>
+    <row r="52" spans="1:13" ht="18.399999999999999" customHeight="1">
+      <c r="A52" s="231" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" s="233"/>
+      <c r="C52" s="227" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="228"/>
       <c r="E52" s="60"/>
-      <c r="F52" s="225" t="s">
+      <c r="F52" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="G52" s="226"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="225" t="s">
+      <c r="G52" s="228"/>
+      <c r="H52" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="I52" s="227" t="s">
         <v>17</v>
       </c>
-      <c r="J52" s="226"/>
+      <c r="J52" s="228"/>
       <c r="K52" s="60"/>
       <c r="L52" s="15"/>
       <c r="M52" s="5"/>
     </row>
     <row r="53" spans="1:13" ht="30">
       <c r="A53" s="78" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B53" s="79" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="C53" s="112">
         <v>1</v>
@@ -4158,7 +4433,9 @@
         <v>2</v>
       </c>
       <c r="E53" s="113"/>
-      <c r="F53" s="109"/>
+      <c r="F53" s="109">
+        <v>1</v>
+      </c>
       <c r="G53" s="110">
         <v>2</v>
       </c>
@@ -4173,10 +4450,10 @@
     </row>
     <row r="54" spans="1:13" ht="30">
       <c r="A54" s="21" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="C54" s="45">
         <v>1</v>
@@ -4185,7 +4462,9 @@
         <v>2</v>
       </c>
       <c r="E54" s="65"/>
-      <c r="F54" s="71"/>
+      <c r="F54" s="71">
+        <v>1</v>
+      </c>
       <c r="G54" s="42">
         <v>2</v>
       </c>
@@ -4200,10 +4479,10 @@
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="56" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="C55" s="45">
         <v>1</v>
@@ -4212,7 +4491,9 @@
         <v>1</v>
       </c>
       <c r="E55" s="65"/>
-      <c r="F55" s="71"/>
+      <c r="F55" s="71">
+        <v>1</v>
+      </c>
       <c r="G55" s="42">
         <v>1</v>
       </c>
@@ -4227,10 +4508,10 @@
     </row>
     <row r="56" spans="1:13" ht="105">
       <c r="A56" s="56" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C56" s="45">
         <v>0.25</v>
@@ -4239,9 +4520,11 @@
         <v>4</v>
       </c>
       <c r="E56" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="F56" s="71"/>
+        <v>134</v>
+      </c>
+      <c r="F56" s="71">
+        <v>1</v>
+      </c>
       <c r="G56" s="42">
         <v>4</v>
       </c>
@@ -4256,10 +4539,10 @@
     </row>
     <row r="57" spans="1:13" ht="45">
       <c r="A57" s="21" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C57" s="45">
         <v>1</v>
@@ -4268,7 +4551,9 @@
         <v>2</v>
       </c>
       <c r="E57" s="65"/>
-      <c r="F57" s="71"/>
+      <c r="F57" s="71">
+        <v>1</v>
+      </c>
       <c r="G57" s="42">
         <v>2</v>
       </c>
@@ -4282,10 +4567,10 @@
       <c r="M57" s="6"/>
     </row>
     <row r="58" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A58" s="227" t="s">
-        <v>32</v>
-      </c>
-      <c r="B58" s="228"/>
+      <c r="A58" s="229" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="230"/>
       <c r="C58" s="98">
         <f>SUMPRODUCT(C53:C57,D53:D57)</f>
         <v>8</v>
@@ -4297,7 +4582,7 @@
       <c r="E58" s="100"/>
       <c r="F58" s="101">
         <f>SUMPRODUCT(F53:F57,G53:G57)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G58" s="102">
         <f>SUM(G53:G57)</f>
@@ -4317,27 +4602,27 @@
       <c r="M58" s="96"/>
     </row>
     <row r="59" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A59" s="253" t="s">
+      <c r="A59" s="255" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="254"/>
-      <c r="C59" s="254"/>
-      <c r="D59" s="254"/>
-      <c r="E59" s="254"/>
-      <c r="F59" s="254"/>
-      <c r="G59" s="254"/>
-      <c r="H59" s="254"/>
-      <c r="I59" s="254"/>
-      <c r="J59" s="254"/>
-      <c r="K59" s="255"/>
+      <c r="B59" s="256"/>
+      <c r="C59" s="256"/>
+      <c r="D59" s="256"/>
+      <c r="E59" s="256"/>
+      <c r="F59" s="256"/>
+      <c r="G59" s="256"/>
+      <c r="H59" s="256"/>
+      <c r="I59" s="256"/>
+      <c r="J59" s="256"/>
+      <c r="K59" s="257"/>
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="256" t="s">
-        <v>119</v>
-      </c>
-      <c r="B60" s="257"/>
+      <c r="A60" s="258" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="259"/>
       <c r="C60" s="133">
         <f t="shared" ref="C60:J60" si="0">C14+C21+C26+C32+C38+C51+C58</f>
         <v>62.7</v>
@@ -4349,7 +4634,7 @@
       <c r="E60" s="64"/>
       <c r="F60" s="134">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70.650000000000006</v>
       </c>
       <c r="G60" s="69">
         <f t="shared" si="0"/>
@@ -4369,28 +4654,28 @@
       <c r="M60" s="6"/>
     </row>
     <row r="61" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A61" s="258" t="s">
-        <v>120</v>
-      </c>
-      <c r="B61" s="259"/>
-      <c r="C61" s="260">
+      <c r="A61" s="260" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" s="261"/>
+      <c r="C61" s="262">
         <f>C60/D60</f>
         <v>0.627</v>
       </c>
-      <c r="D61" s="261"/>
-      <c r="E61" s="262"/>
-      <c r="F61" s="263">
+      <c r="D61" s="263"/>
+      <c r="E61" s="264"/>
+      <c r="F61" s="265">
         <f>F60/G60</f>
-        <v>0</v>
-      </c>
-      <c r="G61" s="264"/>
-      <c r="H61" s="265"/>
-      <c r="I61" s="266">
+        <v>0.70650000000000002</v>
+      </c>
+      <c r="G61" s="266"/>
+      <c r="H61" s="267"/>
+      <c r="I61" s="268">
         <f>I60/J60</f>
         <v>0</v>
       </c>
-      <c r="J61" s="267"/>
-      <c r="K61" s="268"/>
+      <c r="J61" s="269"/>
+      <c r="K61" s="270"/>
       <c r="L61" s="136"/>
       <c r="M61" s="136"/>
     </row>
@@ -4465,8 +4750,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4480,15 +4765,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="269" t="s">
+      <c r="A2" s="271" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="269"/>
-      <c r="C2" s="269"/>
-      <c r="D2" s="269"/>
-      <c r="E2" s="269"/>
-      <c r="F2" s="269"/>
-      <c r="G2" s="269"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="139"/>
@@ -4501,7 +4786,7 @@
     </row>
     <row r="4" spans="1:7" ht="18.75">
       <c r="A4" s="137" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B4" s="137"/>
       <c r="C4" s="137"/>
@@ -4512,42 +4797,42 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:7" ht="24" thickBot="1">
-      <c r="A6" s="277" t="s">
+      <c r="A6" s="279" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="278"/>
-      <c r="C6" s="278"/>
-      <c r="D6" s="278"/>
-      <c r="E6" s="278"/>
-      <c r="F6" s="278"/>
-      <c r="G6" s="279"/>
+      <c r="B6" s="280"/>
+      <c r="C6" s="280"/>
+      <c r="D6" s="280"/>
+      <c r="E6" s="280"/>
+      <c r="F6" s="280"/>
+      <c r="G6" s="281"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="161" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="280"/>
-      <c r="C7" s="280"/>
-      <c r="D7" s="280"/>
-      <c r="E7" s="280"/>
-      <c r="F7" s="280"/>
-      <c r="G7" s="281"/>
+        <v>140</v>
+      </c>
+      <c r="B7" s="282"/>
+      <c r="C7" s="282"/>
+      <c r="D7" s="282"/>
+      <c r="E7" s="282"/>
+      <c r="F7" s="282"/>
+      <c r="G7" s="283"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="208" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B8" s="189" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="189" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="D8" s="189" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="189" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="F8" s="189" t="s">
         <v>17</v>
@@ -4558,7 +4843,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="148" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="B9" s="141">
         <v>1</v>
@@ -4574,13 +4859,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="141" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="G9" s="149"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="191" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="B10" s="192">
         <v>1</v>
@@ -4596,13 +4881,13 @@
         <v>5</v>
       </c>
       <c r="F10" s="192" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="G10" s="193"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="148" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="B11" s="141">
         <v>1</v>
@@ -4618,15 +4903,15 @@
         <v>18</v>
       </c>
       <c r="F11" s="141" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="G11" s="149" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="191" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="B12" s="192">
         <v>1</v>
@@ -4642,13 +4927,13 @@
         <v>16</v>
       </c>
       <c r="F12" s="141" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="G12" s="222"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="148" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="B13" s="141">
         <v>1</v>
@@ -4664,13 +4949,13 @@
         <v>10</v>
       </c>
       <c r="F13" s="141" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="G13" s="149"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="148" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="B14" s="141">
         <v>1</v>
@@ -4686,13 +4971,13 @@
         <v>8</v>
       </c>
       <c r="F14" s="141" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="G14" s="149"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="191" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="B15" s="192">
         <v>1</v>
@@ -4708,13 +4993,13 @@
         <v>12</v>
       </c>
       <c r="F15" s="192" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="G15" s="222"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="148" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B16" s="141">
         <v>1</v>
@@ -4730,13 +5015,13 @@
         <v>10</v>
       </c>
       <c r="F16" s="141" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="G16" s="149"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="191" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B17" s="192">
         <v>1</v>
@@ -4752,13 +5037,13 @@
         <v>4</v>
       </c>
       <c r="F17" s="192" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="G17" s="193"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="148" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="B18" s="141">
         <v>1</v>
@@ -4774,13 +5059,13 @@
         <v>6</v>
       </c>
       <c r="F18" s="141" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="G18" s="149"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="191" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B19" s="192">
         <v>1</v>
@@ -4796,16 +5081,16 @@
         <v>6</v>
       </c>
       <c r="F19" s="192" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="G19" s="193"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="171" t="s">
-        <v>140</v>
-      </c>
-      <c r="B20" s="282"/>
-      <c r="C20" s="282"/>
+        <v>156</v>
+      </c>
+      <c r="B20" s="284"/>
+      <c r="C20" s="284"/>
       <c r="D20" s="221">
         <f>SUM(D9:D19)</f>
         <v>100</v>
@@ -4819,7 +5104,7 @@
     </row>
     <row r="21" spans="1:7" ht="90">
       <c r="A21" s="191" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B21" s="194"/>
       <c r="C21" s="194"/>
@@ -4830,15 +5115,15 @@
         <v>0.25</v>
       </c>
       <c r="F21" s="192" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="G21" s="223" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1">
       <c r="A22" s="150" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="B22" s="151"/>
       <c r="C22" s="151"/>
@@ -4850,42 +5135,42 @@
       <c r="G22" s="153"/>
     </row>
     <row r="23" spans="1:7" ht="24" thickBot="1">
-      <c r="A23" s="283" t="s">
+      <c r="A23" s="285" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="284"/>
-      <c r="C23" s="284"/>
-      <c r="D23" s="284"/>
-      <c r="E23" s="284"/>
-      <c r="F23" s="284"/>
-      <c r="G23" s="285"/>
+      <c r="B23" s="286"/>
+      <c r="C23" s="286"/>
+      <c r="D23" s="286"/>
+      <c r="E23" s="286"/>
+      <c r="F23" s="286"/>
+      <c r="G23" s="287"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="160" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="270"/>
-      <c r="C24" s="270"/>
-      <c r="D24" s="270"/>
-      <c r="E24" s="270"/>
-      <c r="F24" s="270"/>
-      <c r="G24" s="271"/>
+        <v>140</v>
+      </c>
+      <c r="B24" s="272"/>
+      <c r="C24" s="272"/>
+      <c r="D24" s="272"/>
+      <c r="E24" s="272"/>
+      <c r="F24" s="272"/>
+      <c r="G24" s="273"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="207" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B25" s="195" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="195" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="D25" s="195" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="195" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="F25" s="195" t="s">
         <v>17</v>
@@ -4894,209 +5179,233 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="30">
       <c r="A26" s="154" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="B26" s="142">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C26" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="142">
         <v>24</v>
       </c>
       <c r="E26" s="142">
         <f>B26*C26*D26</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="142"/>
-      <c r="G26" s="162"/>
-    </row>
-    <row r="27" spans="1:7">
+        <v>22.799999999999997</v>
+      </c>
+      <c r="F26" s="142" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" s="162" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30">
       <c r="A27" s="197" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="B27" s="198">
-        <v>0</v>
-      </c>
-      <c r="C27" s="198">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="142">
+        <v>1</v>
       </c>
       <c r="D27" s="198">
         <v>8</v>
       </c>
       <c r="E27" s="198">
         <f t="shared" ref="E27:E35" si="1">B27*C27*D27</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="198"/>
+        <v>8</v>
+      </c>
+      <c r="F27" s="142" t="s">
+        <v>161</v>
+      </c>
       <c r="G27" s="199"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="30">
       <c r="A28" s="154" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B28" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="142">
         <v>10</v>
       </c>
       <c r="E28" s="142">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="142"/>
-      <c r="G28" s="162"/>
+        <v>10</v>
+      </c>
+      <c r="F28" s="142" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" s="226" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30">
       <c r="A29" s="197" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="B29" s="198">
-        <v>0</v>
-      </c>
-      <c r="C29" s="198">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C29" s="142">
+        <v>1</v>
       </c>
       <c r="D29" s="198">
         <v>8</v>
       </c>
       <c r="E29" s="198">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="198"/>
+        <v>8</v>
+      </c>
+      <c r="F29" s="142" t="s">
+        <v>161</v>
+      </c>
       <c r="G29" s="199"/>
     </row>
     <row r="30" spans="1:7" ht="30">
       <c r="A30" s="154" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="B30" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="142">
         <v>10</v>
       </c>
       <c r="E30" s="142">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="142"/>
+        <v>10</v>
+      </c>
+      <c r="F30" s="142" t="s">
+        <v>161</v>
+      </c>
       <c r="G30" s="162"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="30">
       <c r="A31" s="197" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="B31" s="198">
-        <v>0</v>
-      </c>
-      <c r="C31" s="198">
-        <v>0</v>
+        <v>0.9</v>
+      </c>
+      <c r="C31" s="142">
+        <v>1</v>
       </c>
       <c r="D31" s="198">
         <v>12</v>
       </c>
       <c r="E31" s="198">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="198"/>
-      <c r="G31" s="199"/>
-    </row>
-    <row r="32" spans="1:7">
+        <v>10.8</v>
+      </c>
+      <c r="F31" s="142" t="s">
+        <v>161</v>
+      </c>
+      <c r="G31" s="225" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30">
       <c r="A32" s="154" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="B32" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="142">
         <v>10</v>
       </c>
       <c r="E32" s="142">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="142"/>
+        <v>10</v>
+      </c>
+      <c r="F32" s="142" t="s">
+        <v>161</v>
+      </c>
       <c r="G32" s="162"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" ht="30">
       <c r="A33" s="197" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="B33" s="198">
-        <v>0</v>
-      </c>
-      <c r="C33" s="198">
-        <v>0</v>
+        <v>0.8</v>
+      </c>
+      <c r="C33" s="142">
+        <v>1</v>
       </c>
       <c r="D33" s="198">
         <v>4</v>
       </c>
       <c r="E33" s="198">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="198"/>
-      <c r="G33" s="199"/>
+        <v>3.2</v>
+      </c>
+      <c r="F33" s="142" t="s">
+        <v>161</v>
+      </c>
+      <c r="G33" s="225" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="154" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="B34" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="142">
         <v>10</v>
       </c>
       <c r="E34" s="142">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F34" s="142"/>
       <c r="G34" s="162"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="154" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="B35" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="142">
         <v>4</v>
       </c>
       <c r="E35" s="142">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F35" s="142"/>
       <c r="G35" s="162"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="167" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="B36" s="168"/>
       <c r="C36" s="168"/>
@@ -5106,14 +5415,14 @@
       </c>
       <c r="E36" s="169">
         <f>SUM(E26:E35)/D36 + E37*D37 + E38*D38 + E39*D39</f>
-        <v>0</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="F36" s="169"/>
       <c r="G36" s="170"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="197" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B37" s="200"/>
       <c r="C37" s="200"/>
@@ -5126,7 +5435,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="154" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="B38" s="143"/>
       <c r="C38" s="143"/>
@@ -5139,7 +5448,7 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1">
       <c r="A39" s="203" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="B39" s="204"/>
       <c r="C39" s="204"/>
@@ -5151,42 +5460,42 @@
       <c r="G39" s="206"/>
     </row>
     <row r="40" spans="1:7" ht="24" thickBot="1">
-      <c r="A40" s="272" t="s">
+      <c r="A40" s="274" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="273"/>
-      <c r="C40" s="273"/>
-      <c r="D40" s="273"/>
-      <c r="E40" s="273"/>
-      <c r="F40" s="273"/>
-      <c r="G40" s="274"/>
+      <c r="B40" s="275"/>
+      <c r="C40" s="275"/>
+      <c r="D40" s="275"/>
+      <c r="E40" s="275"/>
+      <c r="F40" s="275"/>
+      <c r="G40" s="276"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="159" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" s="275"/>
-      <c r="C41" s="275"/>
-      <c r="D41" s="275"/>
-      <c r="E41" s="275"/>
-      <c r="F41" s="275"/>
-      <c r="G41" s="276"/>
+        <v>140</v>
+      </c>
+      <c r="B41" s="277"/>
+      <c r="C41" s="277"/>
+      <c r="D41" s="277"/>
+      <c r="E41" s="277"/>
+      <c r="F41" s="277"/>
+      <c r="G41" s="278"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="178" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B42" s="179" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="179" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="D42" s="179" t="s">
         <v>4</v>
       </c>
       <c r="E42" s="179" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="F42" s="180" t="s">
         <v>17</v>
@@ -5197,7 +5506,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="156" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="B43" s="145">
         <v>0</v>
@@ -5217,7 +5526,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="175" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="B44" s="176">
         <v>0</v>
@@ -5237,7 +5546,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="156" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="B45" s="145">
         <v>0</v>
@@ -5257,7 +5566,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="175" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="B46" s="176">
         <v>0</v>
@@ -5277,7 +5586,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="156" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="B47" s="145">
         <v>0</v>
@@ -5297,7 +5606,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="175" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="B48" s="176">
         <v>0</v>
@@ -5317,7 +5626,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="156" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="B49" s="145">
         <v>0</v>
@@ -5337,7 +5646,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="175" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="B50" s="176">
         <v>0</v>
@@ -5357,7 +5666,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="156" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="B51" s="145">
         <v>0</v>
@@ -5377,7 +5686,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="175" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="B52" s="176">
         <v>0</v>
@@ -5397,7 +5706,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="163" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="B53" s="164"/>
       <c r="C53" s="164"/>
@@ -5414,7 +5723,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="175" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B54" s="182"/>
       <c r="C54" s="182"/>
@@ -5427,7 +5736,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="156" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="B55" s="146"/>
       <c r="C55" s="146"/>
@@ -5440,7 +5749,7 @@
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1">
       <c r="A56" s="185" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="B56" s="186"/>
       <c r="C56" s="186"/>
@@ -5477,6 +5786,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ajout de la note d'UX
</commit_message>
<xml_diff>
--- a/Equipe202.xlsx
+++ b/Equipe202.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24806"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="348" documentId="8_{50A2320D-A701-4D43-9EC9-8C1EC60D081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A85FE5B-F193-4FD3-8524-7D0AC833DC21}"/>
+  <xr:revisionPtr revIDLastSave="349" documentId="8_{50A2320D-A701-4D43-9EC9-8C1EC60D081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9AA7BCB-654A-4E5C-95FE-3B1DED2C616B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="9" r:id="rId1"/>
@@ -2105,138 +2105,138 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="8" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="8" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="9" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="9" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="10" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="10" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="8" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="8" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="9" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="9" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="10" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="10" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2290,13 +2290,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
-    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
-    <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="40 % - Accent2" xfId="5" builtinId="35"/>
+    <cellStyle name="40 % - Accent3" xfId="6" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="3" builtinId="21"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="Sortie" xfId="3" builtinId="21"/>
+    <cellStyle name="Texte explicatif" xfId="2" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2775,8 +2775,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2887,13 +2887,15 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="14"/>
+      <c r="D7" s="14">
+        <v>0.92</v>
+      </c>
       <c r="F7" s="2">
         <v>10</v>
       </c>
       <c r="G7" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.2000000000000011</v>
       </c>
     </row>
   </sheetData>
@@ -2906,7 +2908,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -2926,36 +2928,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A2" s="248" t="s">
+      <c r="A2" s="254" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="248"/>
-      <c r="C2" s="248"/>
-      <c r="D2" s="248"/>
-      <c r="E2" s="248"/>
-      <c r="F2" s="248"/>
-      <c r="G2" s="248"/>
-      <c r="H2" s="248"/>
-      <c r="I2" s="248"/>
-      <c r="J2" s="248"/>
-      <c r="K2" s="248"/>
+      <c r="B2" s="254"/>
+      <c r="C2" s="254"/>
+      <c r="D2" s="254"/>
+      <c r="E2" s="254"/>
+      <c r="F2" s="254"/>
+      <c r="G2" s="254"/>
+      <c r="H2" s="254"/>
+      <c r="I2" s="254"/>
+      <c r="J2" s="254"/>
+      <c r="K2" s="254"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
     </row>
     <row r="4" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A4" s="249" t="s">
+      <c r="A4" s="255" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="249"/>
-      <c r="C4" s="249"/>
-      <c r="D4" s="249"/>
-      <c r="E4" s="249"/>
-      <c r="F4" s="249"/>
-      <c r="G4" s="249"/>
-      <c r="H4" s="249"/>
-      <c r="I4" s="249"/>
-      <c r="J4" s="249"/>
-      <c r="K4" s="249"/>
+      <c r="B4" s="255"/>
+      <c r="C4" s="255"/>
+      <c r="D4" s="255"/>
+      <c r="E4" s="255"/>
+      <c r="F4" s="255"/>
+      <c r="G4" s="255"/>
+      <c r="H4" s="255"/>
+      <c r="I4" s="255"/>
+      <c r="J4" s="255"/>
+      <c r="K4" s="255"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
@@ -2975,36 +2977,36 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A6" s="241" t="s">
+      <c r="A6" s="247" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="253" t="s">
+      <c r="B6" s="259" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="243" t="s">
+      <c r="C6" s="249" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="244"/>
-      <c r="E6" s="244"/>
-      <c r="F6" s="245" t="s">
+      <c r="D6" s="250"/>
+      <c r="E6" s="250"/>
+      <c r="F6" s="251" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="246"/>
-      <c r="H6" s="247"/>
-      <c r="I6" s="250" t="s">
+      <c r="G6" s="252"/>
+      <c r="H6" s="253"/>
+      <c r="I6" s="256" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="251"/>
-      <c r="K6" s="252"/>
+      <c r="J6" s="257"/>
+      <c r="K6" s="258"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="239"/>
-      <c r="O6" s="240"/>
-      <c r="P6" s="240"/>
+      <c r="N6" s="245"/>
+      <c r="O6" s="246"/>
+      <c r="P6" s="246"/>
     </row>
     <row r="7" spans="1:17" ht="19.5" thickBot="1">
-      <c r="A7" s="242"/>
-      <c r="B7" s="254"/>
+      <c r="A7" s="248"/>
+      <c r="B7" s="260"/>
       <c r="C7" s="22" t="s">
         <v>14</v>
       </c>
@@ -3040,26 +3042,26 @@
       <c r="Q7" s="219"/>
     </row>
     <row r="8" spans="1:17" s="20" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A8" s="231" t="s">
+      <c r="A8" s="234" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="232"/>
-      <c r="C8" s="227" t="s">
+      <c r="B8" s="265"/>
+      <c r="C8" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="228"/>
+      <c r="D8" s="270"/>
       <c r="E8" s="60"/>
-      <c r="F8" s="227" t="s">
+      <c r="F8" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="228"/>
+      <c r="G8" s="270"/>
       <c r="H8" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="227" t="s">
+      <c r="I8" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="228"/>
+      <c r="J8" s="270"/>
       <c r="K8" s="60"/>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
@@ -3224,10 +3226,10 @@
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:17" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A14" s="229" t="s">
+      <c r="A14" s="261" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="230"/>
+      <c r="B14" s="262"/>
       <c r="C14" s="87">
         <f>SUMPRODUCT(C9:C13,D9:D13)</f>
         <v>9.5</v>
@@ -3259,26 +3261,26 @@
       <c r="M14" s="96"/>
     </row>
     <row r="15" spans="1:17" s="20" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A15" s="236" t="s">
+      <c r="A15" s="266" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="237"/>
-      <c r="C15" s="227" t="s">
+      <c r="B15" s="267"/>
+      <c r="C15" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="228"/>
+      <c r="D15" s="270"/>
       <c r="E15" s="60"/>
-      <c r="F15" s="227" t="s">
+      <c r="F15" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="228"/>
+      <c r="G15" s="270"/>
       <c r="H15" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="227" t="s">
+      <c r="I15" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="228"/>
+      <c r="J15" s="270"/>
       <c r="K15" s="60"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
@@ -3443,10 +3445,10 @@
       <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A21" s="238" t="s">
+      <c r="A21" s="268" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="235"/>
+      <c r="B21" s="264"/>
       <c r="C21" s="98">
         <f>SUMPRODUCT(C16:C20,D16:D20)</f>
         <v>5.9</v>
@@ -3478,26 +3480,26 @@
       <c r="M21" s="96"/>
     </row>
     <row r="22" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A22" s="231" t="s">
+      <c r="A22" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="232"/>
-      <c r="C22" s="227" t="s">
+      <c r="B22" s="265"/>
+      <c r="C22" s="269" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="228"/>
+      <c r="D22" s="270"/>
       <c r="E22" s="60"/>
-      <c r="F22" s="227" t="s">
+      <c r="F22" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="228"/>
+      <c r="G22" s="270"/>
       <c r="H22" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="I22" s="227" t="s">
+      <c r="I22" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="228"/>
+      <c r="J22" s="270"/>
       <c r="K22" s="60"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
@@ -3596,10 +3598,10 @@
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A26" s="234" t="s">
+      <c r="A26" s="263" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="235"/>
+      <c r="B26" s="264"/>
       <c r="C26" s="87">
         <f>SUMPRODUCT(C23:C25,D23:D25)</f>
         <v>2</v>
@@ -3631,26 +3633,26 @@
       <c r="M26" s="96"/>
     </row>
     <row r="27" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A27" s="231" t="s">
+      <c r="A27" s="234" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="232"/>
-      <c r="C27" s="227" t="s">
+      <c r="B27" s="265"/>
+      <c r="C27" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="228"/>
+      <c r="D27" s="270"/>
       <c r="E27" s="60"/>
-      <c r="F27" s="227" t="s">
+      <c r="F27" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="228"/>
+      <c r="G27" s="270"/>
       <c r="H27" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="227" t="s">
+      <c r="I27" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="228"/>
+      <c r="J27" s="270"/>
       <c r="K27" s="60"/>
       <c r="L27" s="16"/>
       <c r="M27" s="5"/>
@@ -3774,10 +3776,10 @@
       <c r="M31" s="6"/>
     </row>
     <row r="32" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A32" s="229" t="s">
+      <c r="A32" s="261" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="230"/>
+      <c r="B32" s="262"/>
       <c r="C32" s="87">
         <f>SUMPRODUCT(C28:C31,D28:D31)</f>
         <v>6</v>
@@ -3809,19 +3811,19 @@
       <c r="M32" s="96"/>
     </row>
     <row r="33" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A33" s="231" t="s">
+      <c r="A33" s="234" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="233"/>
-      <c r="C33" s="227" t="s">
+      <c r="B33" s="235"/>
+      <c r="C33" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="228"/>
+      <c r="D33" s="270"/>
       <c r="E33" s="60"/>
-      <c r="F33" s="227" t="s">
+      <c r="F33" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="228"/>
+      <c r="G33" s="270"/>
       <c r="H33" s="60" t="s">
         <v>18</v>
       </c>
@@ -3958,10 +3960,10 @@
       <c r="M37" s="6"/>
     </row>
     <row r="38" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A38" s="229" t="s">
+      <c r="A38" s="261" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="230"/>
+      <c r="B38" s="262"/>
       <c r="C38" s="122">
         <f>SUMPRODUCT(C34:C37,D34:D37)</f>
         <v>6.5</v>
@@ -3993,26 +3995,26 @@
       <c r="M38" s="96"/>
     </row>
     <row r="39" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A39" s="231" t="s">
+      <c r="A39" s="234" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="232"/>
-      <c r="C39" s="227" t="s">
+      <c r="B39" s="265"/>
+      <c r="C39" s="269" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="228"/>
+      <c r="D39" s="270"/>
       <c r="E39" s="59"/>
-      <c r="F39" s="227" t="s">
+      <c r="F39" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="228"/>
+      <c r="G39" s="270"/>
       <c r="H39" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="I39" s="227" t="s">
+      <c r="I39" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="J39" s="228"/>
+      <c r="J39" s="270"/>
       <c r="K39" s="60"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
@@ -4360,10 +4362,10 @@
       <c r="M50" s="6"/>
     </row>
     <row r="51" spans="1:13" s="97" customFormat="1" ht="15.75">
-      <c r="A51" s="229" t="s">
+      <c r="A51" s="261" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="230"/>
+      <c r="B51" s="262"/>
       <c r="C51" s="132">
         <f>SUMPRODUCT(C40:C50,D40:D50)</f>
         <v>24.8</v>
@@ -4395,26 +4397,26 @@
       <c r="M51" s="96"/>
     </row>
     <row r="52" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A52" s="231" t="s">
+      <c r="A52" s="234" t="s">
         <v>125</v>
       </c>
-      <c r="B52" s="233"/>
-      <c r="C52" s="227" t="s">
+      <c r="B52" s="235"/>
+      <c r="C52" s="269" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="228"/>
+      <c r="D52" s="270"/>
       <c r="E52" s="60"/>
-      <c r="F52" s="227" t="s">
+      <c r="F52" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="G52" s="228"/>
+      <c r="G52" s="270"/>
       <c r="H52" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="I52" s="227" t="s">
+      <c r="I52" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="J52" s="228"/>
+      <c r="J52" s="270"/>
       <c r="K52" s="60"/>
       <c r="L52" s="15"/>
       <c r="M52" s="5"/>
@@ -4567,10 +4569,10 @@
       <c r="M57" s="6"/>
     </row>
     <row r="58" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A58" s="229" t="s">
+      <c r="A58" s="261" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="230"/>
+      <c r="B58" s="262"/>
       <c r="C58" s="98">
         <f>SUMPRODUCT(C53:C57,D53:D57)</f>
         <v>8</v>
@@ -4602,27 +4604,27 @@
       <c r="M58" s="96"/>
     </row>
     <row r="59" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A59" s="255" t="s">
+      <c r="A59" s="227" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="256"/>
-      <c r="C59" s="256"/>
-      <c r="D59" s="256"/>
-      <c r="E59" s="256"/>
-      <c r="F59" s="256"/>
-      <c r="G59" s="256"/>
-      <c r="H59" s="256"/>
-      <c r="I59" s="256"/>
-      <c r="J59" s="256"/>
-      <c r="K59" s="257"/>
+      <c r="B59" s="228"/>
+      <c r="C59" s="228"/>
+      <c r="D59" s="228"/>
+      <c r="E59" s="228"/>
+      <c r="F59" s="228"/>
+      <c r="G59" s="228"/>
+      <c r="H59" s="228"/>
+      <c r="I59" s="228"/>
+      <c r="J59" s="228"/>
+      <c r="K59" s="229"/>
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="258" t="s">
+      <c r="A60" s="230" t="s">
         <v>137</v>
       </c>
-      <c r="B60" s="259"/>
+      <c r="B60" s="231"/>
       <c r="C60" s="133">
         <f t="shared" ref="C60:J60" si="0">C14+C21+C26+C32+C38+C51+C58</f>
         <v>62.7</v>
@@ -4654,67 +4656,33 @@
       <c r="M60" s="6"/>
     </row>
     <row r="61" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A61" s="260" t="s">
+      <c r="A61" s="232" t="s">
         <v>138</v>
       </c>
-      <c r="B61" s="261"/>
-      <c r="C61" s="262">
+      <c r="B61" s="233"/>
+      <c r="C61" s="236">
         <f>C60/D60</f>
         <v>0.627</v>
       </c>
-      <c r="D61" s="263"/>
-      <c r="E61" s="264"/>
-      <c r="F61" s="265">
+      <c r="D61" s="237"/>
+      <c r="E61" s="238"/>
+      <c r="F61" s="239">
         <f>F60/G60</f>
         <v>0.70650000000000002</v>
       </c>
-      <c r="G61" s="266"/>
-      <c r="H61" s="267"/>
-      <c r="I61" s="268">
+      <c r="G61" s="240"/>
+      <c r="H61" s="241"/>
+      <c r="I61" s="242">
         <f>I60/J60</f>
         <v>0</v>
       </c>
-      <c r="J61" s="269"/>
-      <c r="K61" s="270"/>
+      <c r="J61" s="243"/>
+      <c r="K61" s="244"/>
       <c r="L61" s="136"/>
       <c r="M61" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="I61:K61"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:J15"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="I22:J22"/>
@@ -4729,6 +4697,40 @@
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="I52:J52"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="I61:K61"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L14 L21 L26 L32 L38 L51" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -5791,12 +5793,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5932,13 +5931,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F62C71A-5318-410B-8440-006B73523578}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5946,5 +5948,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F62C71A-5318-410B-8440-006B73523578}"/>
 </file>
</xml_diff>